<commit_message>
merge randomized_method into main: randomize constructive method working, and reports (excel and images working).
</commit_message>
<xml_diff>
--- a/constructive-method/reports/report.xlsx
+++ b/constructive-method/reports/report.xlsx
@@ -512,7 +512,7 @@
         <v>546.3099999999999</v>
       </c>
       <c r="H2" t="n">
-        <v>0.004148960113525391</v>
+        <v>0.002998828887939453</v>
       </c>
     </row>
     <row r="3">
@@ -527,22 +527,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>637.05</v>
+        <v>627.63</v>
       </c>
       <c r="D3" t="n">
-        <v>497.8</v>
+        <v>489.41</v>
       </c>
       <c r="E3" t="n">
-        <v>139.26</v>
+        <v>138.22</v>
       </c>
       <c r="F3" t="n">
-        <v>1134.85</v>
+        <v>1117.04</v>
       </c>
       <c r="G3" t="n">
-        <v>567.42</v>
+        <v>558.52</v>
       </c>
       <c r="H3" t="n">
-        <v>1.818356275558472</v>
+        <v>1.749794721603394</v>
       </c>
     </row>
     <row r="4">
@@ -572,7 +572,7 @@
         <v>504.56</v>
       </c>
       <c r="H4" t="n">
-        <v>0.004072666168212891</v>
+        <v>0.002999305725097656</v>
       </c>
     </row>
     <row r="5">
@@ -587,22 +587,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>515.52</v>
+        <v>514.4</v>
       </c>
       <c r="D5" t="n">
-        <v>515.24</v>
+        <v>514.27</v>
       </c>
       <c r="E5" t="n">
-        <v>0.27</v>
+        <v>0.14</v>
       </c>
       <c r="F5" t="n">
-        <v>1030.76</v>
+        <v>1028.67</v>
       </c>
       <c r="G5" t="n">
-        <v>515.38</v>
+        <v>514.34</v>
       </c>
       <c r="H5" t="n">
-        <v>1.576709508895874</v>
+        <v>1.640929460525513</v>
       </c>
     </row>
     <row r="6">
@@ -632,7 +632,7 @@
         <v>540.9400000000001</v>
       </c>
       <c r="H6" t="n">
-        <v>0.007998943328857422</v>
+        <v>0.006999492645263672</v>
       </c>
     </row>
     <row r="7">
@@ -647,22 +647,22 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>553.34</v>
+        <v>555.95</v>
       </c>
       <c r="D7" t="n">
-        <v>551.79</v>
+        <v>553.0700000000001</v>
       </c>
       <c r="E7" t="n">
-        <v>1.55</v>
+        <v>2.88</v>
       </c>
       <c r="F7" t="n">
-        <v>1658.47</v>
+        <v>1664.91</v>
       </c>
       <c r="G7" t="n">
-        <v>552.8200000000001</v>
+        <v>554.97</v>
       </c>
       <c r="H7" t="n">
-        <v>3.591610908508301</v>
+        <v>3.689326286315918</v>
       </c>
     </row>
     <row r="8">
@@ -692,7 +692,7 @@
         <v>564.01</v>
       </c>
       <c r="H8" t="n">
-        <v>0.01200103759765625</v>
+        <v>0.01099991798400879</v>
       </c>
     </row>
     <row r="9">
@@ -707,22 +707,22 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>686.13</v>
+        <v>690.84</v>
       </c>
       <c r="D9" t="n">
-        <v>451.12</v>
+        <v>469.68</v>
       </c>
       <c r="E9" t="n">
-        <v>235.01</v>
+        <v>221.16</v>
       </c>
       <c r="F9" t="n">
-        <v>2337.62</v>
+        <v>2331.17</v>
       </c>
       <c r="G9" t="n">
-        <v>584.4</v>
+        <v>582.79</v>
       </c>
       <c r="H9" t="n">
-        <v>6.310462951660156</v>
+        <v>6.423193216323853</v>
       </c>
     </row>
     <row r="10">
@@ -752,7 +752,7 @@
         <v>521.63</v>
       </c>
       <c r="H10" t="n">
-        <v>0.01099801063537598</v>
+        <v>0.01000046730041504</v>
       </c>
     </row>
     <row r="11">
@@ -767,22 +767,22 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>538.63</v>
+        <v>537.59</v>
       </c>
       <c r="D11" t="n">
-        <v>525.78</v>
+        <v>530.78</v>
       </c>
       <c r="E11" t="n">
-        <v>12.85</v>
+        <v>6.81</v>
       </c>
       <c r="F11" t="n">
-        <v>2137.03</v>
+        <v>2136.53</v>
       </c>
       <c r="G11" t="n">
-        <v>534.26</v>
+        <v>534.13</v>
       </c>
       <c r="H11" t="n">
-        <v>6.261222124099731</v>
+        <v>6.032886981964111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
READMEs and heuristic methods name updated
</commit_message>
<xml_diff>
--- a/constructive-method/reports/report.xlsx
+++ b/constructive-method/reports/report.xlsx
@@ -512,7 +512,7 @@
         <v>546.3099999999999</v>
       </c>
       <c r="H2" t="n">
-        <v>0.002998828887939453</v>
+        <v>0.004002571105957031</v>
       </c>
     </row>
     <row r="3">
@@ -527,22 +527,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>627.63</v>
+        <v>644.41</v>
       </c>
       <c r="D3" t="n">
-        <v>489.41</v>
+        <v>469.7</v>
       </c>
       <c r="E3" t="n">
-        <v>138.22</v>
+        <v>174.71</v>
       </c>
       <c r="F3" t="n">
-        <v>1117.04</v>
+        <v>1114.11</v>
       </c>
       <c r="G3" t="n">
-        <v>558.52</v>
+        <v>557.05</v>
       </c>
       <c r="H3" t="n">
-        <v>1.749794721603394</v>
+        <v>1.652802228927612</v>
       </c>
     </row>
     <row r="4">
@@ -572,7 +572,7 @@
         <v>504.56</v>
       </c>
       <c r="H4" t="n">
-        <v>0.002999305725097656</v>
+        <v>0.003083229064941406</v>
       </c>
     </row>
     <row r="5">
@@ -587,22 +587,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>514.4</v>
+        <v>515.71</v>
       </c>
       <c r="D5" t="n">
-        <v>514.27</v>
+        <v>514</v>
       </c>
       <c r="E5" t="n">
-        <v>0.14</v>
+        <v>1.71</v>
       </c>
       <c r="F5" t="n">
-        <v>1028.67</v>
+        <v>1029.71</v>
       </c>
       <c r="G5" t="n">
-        <v>514.34</v>
+        <v>514.86</v>
       </c>
       <c r="H5" t="n">
-        <v>1.640929460525513</v>
+        <v>1.614155054092407</v>
       </c>
     </row>
     <row r="6">
@@ -632,7 +632,7 @@
         <v>540.9400000000001</v>
       </c>
       <c r="H6" t="n">
-        <v>0.006999492645263672</v>
+        <v>0.006043195724487305</v>
       </c>
     </row>
     <row r="7">
@@ -647,22 +647,22 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>555.95</v>
+        <v>555.53</v>
       </c>
       <c r="D7" t="n">
-        <v>553.0700000000001</v>
+        <v>551.71</v>
       </c>
       <c r="E7" t="n">
-        <v>2.88</v>
+        <v>3.82</v>
       </c>
       <c r="F7" t="n">
-        <v>1664.91</v>
+        <v>1661.68</v>
       </c>
       <c r="G7" t="n">
-        <v>554.97</v>
+        <v>553.89</v>
       </c>
       <c r="H7" t="n">
-        <v>3.689326286315918</v>
+        <v>3.694030523300171</v>
       </c>
     </row>
     <row r="8">
@@ -692,7 +692,7 @@
         <v>564.01</v>
       </c>
       <c r="H8" t="n">
-        <v>0.01099991798400879</v>
+        <v>0.0110476016998291</v>
       </c>
     </row>
     <row r="9">
@@ -707,22 +707,22 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>690.84</v>
+        <v>693.99</v>
       </c>
       <c r="D9" t="n">
-        <v>469.68</v>
+        <v>448.81</v>
       </c>
       <c r="E9" t="n">
-        <v>221.16</v>
+        <v>245.18</v>
       </c>
       <c r="F9" t="n">
-        <v>2331.17</v>
+        <v>2334.93</v>
       </c>
       <c r="G9" t="n">
-        <v>582.79</v>
+        <v>583.73</v>
       </c>
       <c r="H9" t="n">
-        <v>6.423193216323853</v>
+        <v>6.131538867950439</v>
       </c>
     </row>
     <row r="10">
@@ -752,7 +752,7 @@
         <v>521.63</v>
       </c>
       <c r="H10" t="n">
-        <v>0.01000046730041504</v>
+        <v>0.01109099388122559</v>
       </c>
     </row>
     <row r="11">
@@ -767,22 +767,22 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>537.59</v>
+        <v>540.41</v>
       </c>
       <c r="D11" t="n">
-        <v>530.78</v>
+        <v>529.09</v>
       </c>
       <c r="E11" t="n">
-        <v>6.81</v>
+        <v>11.32</v>
       </c>
       <c r="F11" t="n">
-        <v>2136.53</v>
+        <v>2145.14</v>
       </c>
       <c r="G11" t="n">
-        <v>534.13</v>
+        <v>536.28</v>
       </c>
       <c r="H11" t="n">
-        <v>6.032886981964111</v>
+        <v>6.246362447738647</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bar chart updated (grouped)
</commit_message>
<xml_diff>
--- a/constructive-method/reports/report.xlsx
+++ b/constructive-method/reports/report.xlsx
@@ -512,7 +512,7 @@
         <v>546.3099999999999</v>
       </c>
       <c r="H2" t="n">
-        <v>0.004002571105957031</v>
+        <v>0.004000186920166016</v>
       </c>
     </row>
     <row r="3">
@@ -527,22 +527,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>644.41</v>
+        <v>640.41</v>
       </c>
       <c r="D3" t="n">
-        <v>469.7</v>
+        <v>493.05</v>
       </c>
       <c r="E3" t="n">
-        <v>174.71</v>
+        <v>147.36</v>
       </c>
       <c r="F3" t="n">
-        <v>1114.11</v>
+        <v>1133.46</v>
       </c>
       <c r="G3" t="n">
-        <v>557.05</v>
+        <v>566.73</v>
       </c>
       <c r="H3" t="n">
-        <v>1.652802228927612</v>
+        <v>1.642164468765259</v>
       </c>
     </row>
     <row r="4">
@@ -572,7 +572,7 @@
         <v>504.56</v>
       </c>
       <c r="H4" t="n">
-        <v>0.003083229064941406</v>
+        <v>0.003081560134887695</v>
       </c>
     </row>
     <row r="5">
@@ -587,22 +587,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>515.71</v>
+        <v>515.24</v>
       </c>
       <c r="D5" t="n">
-        <v>514</v>
+        <v>512.42</v>
       </c>
       <c r="E5" t="n">
-        <v>1.71</v>
+        <v>2.82</v>
       </c>
       <c r="F5" t="n">
-        <v>1029.71</v>
+        <v>1027.66</v>
       </c>
       <c r="G5" t="n">
-        <v>514.86</v>
+        <v>513.83</v>
       </c>
       <c r="H5" t="n">
-        <v>1.614155054092407</v>
+        <v>1.55881142616272</v>
       </c>
     </row>
     <row r="6">
@@ -632,7 +632,7 @@
         <v>540.9400000000001</v>
       </c>
       <c r="H6" t="n">
-        <v>0.006043195724487305</v>
+        <v>0.00599980354309082</v>
       </c>
     </row>
     <row r="7">
@@ -647,22 +647,22 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>555.53</v>
+        <v>555.13</v>
       </c>
       <c r="D7" t="n">
-        <v>551.71</v>
+        <v>549.67</v>
       </c>
       <c r="E7" t="n">
-        <v>3.82</v>
+        <v>5.47</v>
       </c>
       <c r="F7" t="n">
-        <v>1661.68</v>
+        <v>1657.6</v>
       </c>
       <c r="G7" t="n">
-        <v>553.89</v>
+        <v>552.53</v>
       </c>
       <c r="H7" t="n">
-        <v>3.694030523300171</v>
+        <v>3.508722305297852</v>
       </c>
     </row>
     <row r="8">
@@ -692,7 +692,7 @@
         <v>564.01</v>
       </c>
       <c r="H8" t="n">
-        <v>0.0110476016998291</v>
+        <v>0.01004457473754883</v>
       </c>
     </row>
     <row r="9">
@@ -707,22 +707,22 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>693.99</v>
+        <v>700.83</v>
       </c>
       <c r="D9" t="n">
-        <v>448.81</v>
+        <v>454.02</v>
       </c>
       <c r="E9" t="n">
-        <v>245.18</v>
+        <v>246.81</v>
       </c>
       <c r="F9" t="n">
-        <v>2334.93</v>
+        <v>2322.92</v>
       </c>
       <c r="G9" t="n">
-        <v>583.73</v>
+        <v>580.73</v>
       </c>
       <c r="H9" t="n">
-        <v>6.131538867950439</v>
+        <v>6.381536722183228</v>
       </c>
     </row>
     <row r="10">
@@ -752,7 +752,7 @@
         <v>521.63</v>
       </c>
       <c r="H10" t="n">
-        <v>0.01109099388122559</v>
+        <v>0.01105976104736328</v>
       </c>
     </row>
     <row r="11">
@@ -767,22 +767,22 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>540.41</v>
+        <v>540.55</v>
       </c>
       <c r="D11" t="n">
-        <v>529.09</v>
+        <v>530.55</v>
       </c>
       <c r="E11" t="n">
-        <v>11.32</v>
+        <v>10</v>
       </c>
       <c r="F11" t="n">
-        <v>2145.14</v>
+        <v>2140.9</v>
       </c>
       <c r="G11" t="n">
-        <v>536.28</v>
+        <v>535.22</v>
       </c>
       <c r="H11" t="n">
-        <v>6.246362447738647</v>
+        <v>5.761125564575195</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
constructive method and report finished
</commit_message>
<xml_diff>
--- a/constructive-method/reports/report.xlsx
+++ b/constructive-method/reports/report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>40_heterogeneous</t>
+          <t>40_homogeneous</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -497,28 +497,28 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>641.67</v>
+        <v>508.72</v>
       </c>
       <c r="D2" t="n">
-        <v>450.95</v>
+        <v>500.4</v>
       </c>
       <c r="E2" t="n">
-        <v>190.72</v>
+        <v>8.32</v>
       </c>
       <c r="F2" t="n">
-        <v>1092.62</v>
+        <v>1009.12</v>
       </c>
       <c r="G2" t="n">
-        <v>546.3099999999999</v>
+        <v>504.56</v>
       </c>
       <c r="H2" t="n">
-        <v>0.004000186920166016</v>
+        <v>0.003000736236572266</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>40_heterogeneous</t>
+          <t>40_homogeneous</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -527,28 +527,28 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>640.41</v>
+        <v>514.89</v>
       </c>
       <c r="D3" t="n">
-        <v>493.05</v>
+        <v>513.13</v>
       </c>
       <c r="E3" t="n">
-        <v>147.36</v>
+        <v>1.75</v>
       </c>
       <c r="F3" t="n">
-        <v>1133.46</v>
+        <v>1028.02</v>
       </c>
       <c r="G3" t="n">
-        <v>566.73</v>
+        <v>514.01</v>
       </c>
       <c r="H3" t="n">
-        <v>1.642164468765259</v>
+        <v>1.670448303222656</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>40_homogeneous</t>
+          <t>40_heterogeneous</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -557,28 +557,28 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>508.72</v>
+        <v>641.67</v>
       </c>
       <c r="D4" t="n">
-        <v>500.4</v>
+        <v>450.95</v>
       </c>
       <c r="E4" t="n">
-        <v>8.32</v>
+        <v>190.72</v>
       </c>
       <c r="F4" t="n">
-        <v>1009.12</v>
+        <v>1092.62</v>
       </c>
       <c r="G4" t="n">
-        <v>504.56</v>
+        <v>546.3099999999999</v>
       </c>
       <c r="H4" t="n">
-        <v>0.003081560134887695</v>
+        <v>0.002999305725097656</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>40_homogeneous</t>
+          <t>40_heterogeneous</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -587,22 +587,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>515.24</v>
+        <v>641.03</v>
       </c>
       <c r="D5" t="n">
-        <v>512.42</v>
+        <v>480.89</v>
       </c>
       <c r="E5" t="n">
-        <v>2.82</v>
+        <v>160.14</v>
       </c>
       <c r="F5" t="n">
-        <v>1027.66</v>
+        <v>1121.93</v>
       </c>
       <c r="G5" t="n">
-        <v>513.83</v>
+        <v>560.96</v>
       </c>
       <c r="H5" t="n">
-        <v>1.55881142616272</v>
+        <v>1.758956670761108</v>
       </c>
     </row>
     <row r="6">
@@ -632,7 +632,7 @@
         <v>540.9400000000001</v>
       </c>
       <c r="H6" t="n">
-        <v>0.00599980354309082</v>
+        <v>0.01012277603149414</v>
       </c>
     </row>
     <row r="7">
@@ -647,28 +647,28 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>555.13</v>
+        <v>556.29</v>
       </c>
       <c r="D7" t="n">
-        <v>549.67</v>
+        <v>547.04</v>
       </c>
       <c r="E7" t="n">
-        <v>5.47</v>
+        <v>9.25</v>
       </c>
       <c r="F7" t="n">
-        <v>1657.6</v>
+        <v>1657.63</v>
       </c>
       <c r="G7" t="n">
-        <v>552.53</v>
+        <v>552.54</v>
       </c>
       <c r="H7" t="n">
-        <v>3.508722305297852</v>
+        <v>3.73978066444397</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>80_heterogeneous</t>
+          <t>60_heterogeneous</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -677,28 +677,28 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>670.96</v>
+        <v>631.05</v>
       </c>
       <c r="D8" t="n">
-        <v>456.45</v>
+        <v>491.1</v>
       </c>
       <c r="E8" t="n">
-        <v>214.51</v>
+        <v>139.95</v>
       </c>
       <c r="F8" t="n">
-        <v>2256.02</v>
+        <v>1746.6</v>
       </c>
       <c r="G8" t="n">
-        <v>564.01</v>
+        <v>582.2</v>
       </c>
       <c r="H8" t="n">
-        <v>0.01004457473754883</v>
+        <v>0.01000070571899414</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>80_heterogeneous</t>
+          <t>60_heterogeneous</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -707,22 +707,22 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>700.83</v>
+        <v>652.01</v>
       </c>
       <c r="D9" t="n">
-        <v>454.02</v>
+        <v>509.49</v>
       </c>
       <c r="E9" t="n">
-        <v>246.81</v>
+        <v>142.52</v>
       </c>
       <c r="F9" t="n">
-        <v>2322.92</v>
+        <v>1807.74</v>
       </c>
       <c r="G9" t="n">
-        <v>580.73</v>
+        <v>602.58</v>
       </c>
       <c r="H9" t="n">
-        <v>6.381536722183228</v>
+        <v>4.066461801528931</v>
       </c>
     </row>
     <row r="10">
@@ -752,7 +752,7 @@
         <v>521.63</v>
       </c>
       <c r="H10" t="n">
-        <v>0.01105976104736328</v>
+        <v>0.01059842109680176</v>
       </c>
     </row>
     <row r="11">
@@ -767,22 +767,82 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>540.55</v>
+        <v>541</v>
       </c>
       <c r="D11" t="n">
-        <v>530.55</v>
+        <v>536.12</v>
       </c>
       <c r="E11" t="n">
-        <v>10</v>
+        <v>4.88</v>
       </c>
       <c r="F11" t="n">
-        <v>2140.9</v>
+        <v>2156.28</v>
       </c>
       <c r="G11" t="n">
-        <v>535.22</v>
+        <v>539.0700000000001</v>
       </c>
       <c r="H11" t="n">
-        <v>5.761125564575195</v>
+        <v>6.165876150131226</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>80_heterogeneous</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>deterministic</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>670.96</v>
+      </c>
+      <c r="D12" t="n">
+        <v>456.45</v>
+      </c>
+      <c r="E12" t="n">
+        <v>214.51</v>
+      </c>
+      <c r="F12" t="n">
+        <v>2256.02</v>
+      </c>
+      <c r="G12" t="n">
+        <v>564.01</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.01103901863098145</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>80_heterogeneous</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>randomized</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>693.26</v>
+      </c>
+      <c r="D13" t="n">
+        <v>442.47</v>
+      </c>
+      <c r="E13" t="n">
+        <v>250.79</v>
+      </c>
+      <c r="F13" t="n">
+        <v>2346.15</v>
+      </c>
+      <c r="G13" t="n">
+        <v>586.54</v>
+      </c>
+      <c r="H13" t="n">
+        <v>6.475290536880493</v>
       </c>
     </row>
   </sheetData>

</xml_diff>